<commit_message>
add base data op
</commit_message>
<xml_diff>
--- a/docs/v2.0/示例.xlsx
+++ b/docs/v2.0/示例.xlsx
@@ -1,35 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huizi/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="760" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
     <sheet name="property" sheetId="2" r:id="rId2"/>
     <sheet name="config" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
   <si>
     <t>ID</t>
   </si>
@@ -43,239 +30,550 @@
     <t>type</t>
   </si>
   <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>chassis</t>
+  </si>
+  <si>
+    <t>fru</t>
+  </si>
+  <si>
+    <t>CPU0_DTS_Temp</t>
+  </si>
+  <si>
+    <t>CPU0_PECI_Value</t>
+  </si>
+  <si>
+    <t>SYS_Air_Inlet</t>
+  </si>
+  <si>
+    <t>MB_Air_Inlet</t>
+  </si>
+  <si>
+    <t>SYS_Air_Outlet</t>
+  </si>
+  <si>
+    <t>Mezz_Card_Area</t>
+  </si>
+  <si>
+    <t>PCH_Temp</t>
+  </si>
+  <si>
+    <t>CPU0_DIMM_C0</t>
+  </si>
+  <si>
+    <t>VCCP_P0</t>
+  </si>
+  <si>
+    <t>VPP_P0</t>
+  </si>
+  <si>
+    <t>CPU0_DTS_Temp/Max</t>
+  </si>
+  <si>
+    <t>CPU0_DTS_Temp/Min</t>
+  </si>
+  <si>
+    <t>mc/Device ID</t>
+  </si>
+  <si>
+    <t>mc/Firmware Revision</t>
+  </si>
+  <si>
+    <t>mc/IPMI Version</t>
+  </si>
+  <si>
+    <t>mc/Manufacturer ID</t>
+  </si>
+  <si>
+    <t>mc/Manufacturer Name</t>
+  </si>
+  <si>
+    <t>mc/Product ID</t>
+  </si>
+  <si>
+    <t>chassis/System Power</t>
+  </si>
+  <si>
+    <t>chassis/Power Restore Policy</t>
+  </si>
+  <si>
+    <t>chassis/Chassis Intrusion</t>
+  </si>
+  <si>
+    <t>chassis/Front-Panel Lockout</t>
+  </si>
+  <si>
+    <t>fru/Board Mfg Date</t>
+  </si>
+  <si>
+    <t>fru/Board Serial</t>
+  </si>
+  <si>
+    <t>fru/Board Product</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>targetid</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>config_id</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>Tyan Computer Corporation</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>always-on</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>Wed Jan 15 18:54:00 2014</t>
+  </si>
+  <si>
+    <t>CGUD1JH0200M</t>
+  </si>
+  <si>
+    <t>57086GM3NR</t>
+  </si>
+  <si>
+    <t>55 degrees C</t>
+  </si>
+  <si>
+    <t>unspecified</t>
+  </si>
+  <si>
+    <t>12 degrees C</t>
+  </si>
+  <si>
+    <t>53 degrees C</t>
+  </si>
+  <si>
+    <t>10 degrees C</t>
+  </si>
+  <si>
+    <t>18 degrees C</t>
+  </si>
+  <si>
+    <t>17 degrees C</t>
+  </si>
+  <si>
+    <t>15 degrees C</t>
+  </si>
+  <si>
+    <t>20 degrees C</t>
+  </si>
+  <si>
+    <t>0 degrees C</t>
+  </si>
+  <si>
+    <t>21 degrees C</t>
+  </si>
+  <si>
+    <t>1.76 Volts</t>
+  </si>
+  <si>
+    <t>2.44 Volts</t>
+  </si>
+  <si>
+    <t>80 degrees C</t>
+  </si>
+  <si>
+    <t>22 degrees C</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>superuser</t>
+  </si>
+  <si>
     <t>192.168.1.3</t>
   </si>
   <si>
     <t>192.168.1.4</t>
-  </si>
-  <si>
-    <t>mc</t>
-  </si>
-  <si>
-    <t>chassis</t>
-  </si>
-  <si>
-    <t>fru</t>
-  </si>
-  <si>
-    <t>CPU0_DTS_Temp</t>
-  </si>
-  <si>
-    <t>CPU0_PECI_Value</t>
-  </si>
-  <si>
-    <t>SYS_Air_Inlet</t>
-  </si>
-  <si>
-    <t>MB_Air_Inlet</t>
-  </si>
-  <si>
-    <t>SYS_Air_Outlet</t>
-  </si>
-  <si>
-    <t>Mezz_Card_Area</t>
-  </si>
-  <si>
-    <t>PCH_Temp</t>
-  </si>
-  <si>
-    <t>CPU0_DIMM_C0</t>
-  </si>
-  <si>
-    <t>VCCP_P0</t>
-  </si>
-  <si>
-    <t>VPP_P0</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>targetid</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>config_id</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>Tyan Computer Corporation</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>always-on</t>
-  </si>
-  <si>
-    <t>inactive</t>
-  </si>
-  <si>
-    <t>Wed Jan 15 18:54:00 2014</t>
-  </si>
-  <si>
-    <t>CGUD1JH0200M</t>
-  </si>
-  <si>
-    <t>57086GM3NR</t>
-  </si>
-  <si>
-    <t>55 degrees C</t>
-  </si>
-  <si>
-    <t>0 degrees C</t>
-  </si>
-  <si>
-    <t>20 degrees C</t>
-  </si>
-  <si>
-    <t>21 degrees C</t>
-  </si>
-  <si>
-    <t>1.76 Volts</t>
-  </si>
-  <si>
-    <t>2.44 Volts</t>
-  </si>
-  <si>
-    <t>17 degrees C</t>
-  </si>
-  <si>
-    <t>18 degrees C</t>
-  </si>
-  <si>
-    <t>12 degrees C</t>
-  </si>
-  <si>
-    <t>unspecified</t>
-  </si>
-  <si>
-    <t>80 degrees C</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>pwd</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>CPU0_DTS_Temp/Max</t>
-  </si>
-  <si>
-    <t>CPU0_DTS_Temp/Min</t>
-  </si>
-  <si>
-    <t>system</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>superuser</t>
-  </si>
-  <si>
-    <t>mc/Device ID</t>
-  </si>
-  <si>
-    <t>mc/Firmware Revision</t>
-  </si>
-  <si>
-    <t>mc/IPMI Version</t>
-  </si>
-  <si>
-    <t>mc/Manufacturer ID</t>
-  </si>
-  <si>
-    <t>mc/Manufacturer Name</t>
-  </si>
-  <si>
-    <t>mc/Product ID</t>
-  </si>
-  <si>
-    <t>chassis/System Power</t>
-  </si>
-  <si>
-    <t>chassis/Power Restore Policy</t>
-  </si>
-  <si>
-    <t>chassis/Chassis Intrusion</t>
-  </si>
-  <si>
-    <t>chassis/Front-Panel Lockout</t>
-  </si>
-  <si>
-    <t>fru/Board Mfg Date</t>
-  </si>
-  <si>
-    <t>fru/Board Serial</t>
-  </si>
-  <si>
-    <t>fru/Board Product</t>
-  </si>
-  <si>
-    <t>53 degrees C</t>
-  </si>
-  <si>
-    <t>10 degrees C</t>
-  </si>
-  <si>
-    <t>15 degrees C</t>
-  </si>
-  <si>
-    <t>22 degrees C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -283,25 +581,298 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="47">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="百分比" xfId="10" builtinId="5"/>
+    <cellStyle name="注释" xfId="11" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="12" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="13" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11"/>
+    <cellStyle name="标题" xfId="15" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="17" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="18" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="19" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="20" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="21" builtinId="44"/>
+    <cellStyle name="输出" xfId="22" builtinId="21"/>
+    <cellStyle name="计算" xfId="23" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="25" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="26" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="27" builtinId="24"/>
+    <cellStyle name="汇总" xfId="28" builtinId="25"/>
+    <cellStyle name="好" xfId="29" builtinId="26"/>
+    <cellStyle name="适中" xfId="30" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="31" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="32" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="33" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="34" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="35" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="36" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="37" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="38" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="39" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="40" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="42" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="43" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="44" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="45" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="46" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -354,7 +925,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -389,7 +960,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -563,32 +1134,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.8333333333333" customWidth="1"/>
+    <col min="2" max="2" width="27.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="25.8333333333333" customWidth="1"/>
     <col min="4" max="4" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,362 +1168,364 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="11.1666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -974,7 +1542,7 @@
         <v>1515682882</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -991,7 +1559,7 @@
         <v>1515682882</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1008,7 +1576,7 @@
         <v>1515682882</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1025,7 +1593,7 @@
         <v>1515682882</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1042,7 +1610,7 @@
         <v>1515682883</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1059,7 +1627,7 @@
         <v>1515682883</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1076,7 +1644,7 @@
         <v>1515682883</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1084,7 +1652,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1093,7 +1661,7 @@
         <v>1515682883</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1101,7 +1669,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1110,7 +1678,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1127,7 +1695,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1135,7 +1703,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1144,7 +1712,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1152,7 +1720,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1161,7 +1729,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1169,7 +1737,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1178,7 +1746,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1186,7 +1754,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1195,7 +1763,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1203,7 +1771,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1212,7 +1780,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1220,7 +1788,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1229,7 +1797,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1237,7 +1805,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1246,7 +1814,7 @@
         <v>1515682885</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1254,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1263,7 +1831,7 @@
         <v>1515682885</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1271,7 +1839,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1280,7 +1848,7 @@
         <v>1515682885</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1288,7 +1856,7 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1297,7 +1865,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1305,7 +1873,7 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1314,7 +1882,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1322,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1331,7 +1899,7 @@
         <v>1515682885</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1339,7 +1907,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1348,7 +1916,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1356,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1365,7 +1933,7 @@
         <v>1515682884</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1373,7 +1941,7 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1382,7 +1950,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1390,7 +1958,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1399,7 +1967,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1407,7 +1975,7 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1416,7 +1984,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1424,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1433,7 +2001,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1441,7 +2009,7 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1450,7 +2018,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1458,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1467,7 +2035,7 @@
         <v>1515682886</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1475,7 +2043,7 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1484,7 +2052,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1492,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -1501,7 +2069,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1509,7 +2077,7 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -1518,7 +2086,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1526,7 +2094,7 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1535,7 +2103,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1543,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -1552,7 +2120,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1560,7 +2128,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1569,7 +2137,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1577,7 +2145,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1586,7 +2154,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1594,7 +2162,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1603,7 +2171,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1611,7 +2179,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1620,7 +2188,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1628,7 +2196,7 @@
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -1637,7 +2205,7 @@
         <v>1515682888</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1645,7 +2213,7 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1655,89 +2223,92 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="3" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>